<commit_message>
Fifth Commit - GRID, Jenkins, GIT, Github
</commit_message>
<xml_diff>
--- a/Excel/loginData.xlsx
+++ b/Excel/loginData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Desktop\SeleniumPython\Workspace_POM\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A13F0D-4B8D-4809-8407-451595BBDAA4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E0CCFC6-9711-486B-B9D9-6DC3EC8F1A5E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1" xr2:uid="{D88BDF0A-0091-42FF-96C3-52E616FC4DB0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="2" xr2:uid="{D88BDF0A-0091-42FF-96C3-52E616FC4DB0}"/>
   </bookViews>
   <sheets>
     <sheet name="SendMail" sheetId="1" r:id="rId1"/>
@@ -473,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7269458D-F869-42CA-A92E-1EB07FC3C95E}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A3" sqref="A3:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -522,41 +522,23 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="selenium.testmay@2017" xr:uid="{F4BF84C9-359C-445C-A1AA-676D33A9DEE6}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{3EDC998E-2EF4-4602-B405-988657B61FC2}"/>
     <hyperlink ref="C2" r:id="rId3" xr:uid="{AECF3495-9453-4867-96DE-1A08381C546D}"/>
-    <hyperlink ref="B3" r:id="rId4" xr:uid="{57348F67-1B33-4FC0-98B6-D08752A20385}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId5"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05334B6A-D7F9-4171-A879-205785D63BE8}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,29 +584,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="selenium.testmay@2017" xr:uid="{51E203ED-856A-4369-9748-5D426CB0CD32}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{730E9FC7-5213-4B5E-B1B7-32BE86D263B6}"/>
     <hyperlink ref="C2" r:id="rId3" xr:uid="{0AFCCA62-5AFF-4D3B-8F1E-C4A5B1339703}"/>
-    <hyperlink ref="B3" r:id="rId4" xr:uid="{D3C5F107-1017-4309-BCC7-7F66CB0E5E6F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -632,14 +596,31 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{173EB1A8-0E54-492B-AF0F-D81EABAFDDA7}">
-  <dimension ref="B3:F6"/>
+  <dimension ref="B2:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+    </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>5</v>
@@ -706,6 +687,23 @@
       </c>
       <c r="F6" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -716,6 +714,8 @@
     <hyperlink ref="C5" r:id="rId4" xr:uid="{5BF0B0C0-E109-43D9-9B0F-38022F348E41}"/>
     <hyperlink ref="C6" r:id="rId5" xr:uid="{F83F6837-FB44-46D8-9453-01ECFE5326F4}"/>
     <hyperlink ref="D6" r:id="rId6" xr:uid="{E1B4BA87-8680-42B5-9165-6DC77BB18051}"/>
+    <hyperlink ref="C7" r:id="rId7" xr:uid="{D3C5F107-1017-4309-BCC7-7F66CB0E5E6F}"/>
+    <hyperlink ref="C2" r:id="rId8" xr:uid="{57348F67-1B33-4FC0-98B6-D08752A20385}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>